<commit_message>
Seleinum IDE pratical file
</commit_message>
<xml_diff>
--- a/Project/Bstack Demo_project.xlsx
+++ b/Project/Bstack Demo_project.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Top's\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66319701-C487-4FFB-B23D-039240EF77AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6ECE7D-E60E-4B13-A84A-3573681BE4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{AE5AE047-C2CA-4AA1-993B-987C52EAEFDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scenario" sheetId="1" r:id="rId1"/>
-    <sheet name="HLR" sheetId="2" r:id="rId2"/>
-    <sheet name="HLR STACK DEMO" sheetId="5" r:id="rId3"/>
-    <sheet name="Test Case" sheetId="3" r:id="rId4"/>
-    <sheet name="Bug Report" sheetId="4" r:id="rId5"/>
+    <sheet name="HLR STACK DEMO" sheetId="5" r:id="rId2"/>
+    <sheet name="Test Case" sheetId="3" r:id="rId3"/>
+    <sheet name="Bug Report" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="147">
   <si>
     <t xml:space="preserve">Bstack Demo </t>
   </si>
@@ -259,147 +258,12 @@
     <t>Try registering with an already existing email and check the system response.</t>
   </si>
   <si>
-    <t>Functionality ID</t>
-  </si>
-  <si>
-    <t>Funcational Name</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Check the website URL</t>
-  </si>
-  <si>
     <t>while enter this url"https://bstackdemo.com/" it should be open the first page</t>
   </si>
   <si>
-    <t>while user click the sign in opetion it should be display the login page</t>
-  </si>
-  <si>
-    <t>Check the login button</t>
-  </si>
-  <si>
-    <t>While user enter the username &amp; password click on login button it should be redirect to the home page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check DEMO </t>
-  </si>
-  <si>
-    <t>While user click on DEMO it should be redirect to the home page.</t>
-  </si>
-  <si>
-    <t>Check the Offers</t>
-  </si>
-  <si>
-    <t>While user click on Offers it should be display the offering page or discount page which mobile phone is more than or less than discount</t>
-  </si>
-  <si>
-    <t>While user click on Favourite it should be open the favourite iteam list.</t>
-  </si>
-  <si>
-    <t>Check the Seach bar</t>
-  </si>
-  <si>
-    <t>While user search the product and enter the search it should be display the product</t>
-  </si>
-  <si>
-    <t>Check the Cart</t>
-  </si>
-  <si>
-    <t>While user click on Cart option it should be display all product when you'r adding the product in add to cart</t>
-  </si>
-  <si>
-    <t>Check the " Checkout"</t>
-  </si>
-  <si>
-    <t>While user click on Checkout it should be redirect to the shipping address page</t>
-  </si>
-  <si>
-    <t>Check the Submit</t>
-  </si>
-  <si>
-    <t>While user full the shipping address with first name, last name, address, state and postal and click on submit button it should be direct go to the confirmation page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check the CONTINUE SHOPPING </t>
-  </si>
-  <si>
-    <t>While user click on continue shopping It should be redirect to the home page.</t>
-  </si>
-  <si>
-    <t>Check the " APPLE" option</t>
-  </si>
-  <si>
-    <t>While user click on APPLE option it should be display the all iphone items</t>
-  </si>
-  <si>
-    <t>Check the " Samsung" Option</t>
-  </si>
-  <si>
-    <t>While user click on Samsung it should be display the all samsung itemas</t>
-  </si>
-  <si>
-    <t>Check the " Google" Option</t>
-  </si>
-  <si>
-    <t>While user click on Google it should be display the all google iteams</t>
-  </si>
-  <si>
-    <t>Check the "OnePlus"</t>
-  </si>
-  <si>
-    <t>While user click on OnePlus it should be display the OnePlus mobile items</t>
-  </si>
-  <si>
-    <t>While user click on Favourite product add to the favourite list</t>
-  </si>
-  <si>
-    <t>Check the " Unfavourite"</t>
-  </si>
-  <si>
-    <t>While user click on unfavourite product remove from the favourite items</t>
-  </si>
-  <si>
-    <t>Check the " Add to Cart"</t>
-  </si>
-  <si>
-    <t>While user click on add to cart product add on the Cart.</t>
-  </si>
-  <si>
-    <t>Check the" Plus(+)"</t>
-  </si>
-  <si>
-    <t>While user click on + it should be increase the product quantity</t>
-  </si>
-  <si>
-    <t>Check the " Minus(-)"</t>
-  </si>
-  <si>
-    <t>While user click on - it should be decrese the product quantity</t>
-  </si>
-  <si>
-    <t>Check the " Order BY filter"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">While user select the order by lower to higher and higher to lower it should be listed the </t>
-  </si>
-  <si>
-    <t>Check the Sign in Button</t>
-  </si>
-  <si>
-    <t>Check the " Favourite icon"</t>
-  </si>
-  <si>
-    <t>Check the Favourites button</t>
-  </si>
-  <si>
-    <t>Check Logout Button</t>
-  </si>
-  <si>
-    <t>While user click on Logout button, it should be logout the account.</t>
-  </si>
-  <si>
     <t>Bstack DEMO</t>
   </si>
   <si>
@@ -500,13 +364,118 @@
   </si>
   <si>
     <t>While user click on " OnePlus" Button it should be display the Oneplus mobile product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on " iPhone 12" </t>
+  </si>
+  <si>
+    <t>While user click on iphone 12 product, it does not open and show the description of product</t>
+  </si>
+  <si>
+    <t>Click on "Add to cart"</t>
+  </si>
+  <si>
+    <t>Click on " Favourite" icon</t>
+  </si>
+  <si>
+    <t>While user click on Favourite it should be product add on the favourite iteam list</t>
+  </si>
+  <si>
+    <t>Click on " iphone 12 mini"</t>
+  </si>
+  <si>
+    <t>While user click on iphone 12 mini product, it does not open and not show the description of product</t>
+  </si>
+  <si>
+    <t>Click on " Add to cart" button</t>
+  </si>
+  <si>
+    <t>while user click on add to cart it should be product move on the Bag</t>
+  </si>
+  <si>
+    <t>While user click on " Add to cart" button it should be product move on the the Bag</t>
+  </si>
+  <si>
+    <t>Check the Favourite feature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When user add the product in favourite list then change the vendor suppose where select the samsung vendor then user click on favourites button/ go to the favourite list it does not show the favourite product item </t>
+  </si>
+  <si>
+    <t>Check the order by</t>
+  </si>
+  <si>
+    <t>while user select the lowest to highest, product item change the lower to higher price product</t>
+  </si>
+  <si>
+    <t>While user select the highest to lowest, it should be change the higher to lower price product</t>
+  </si>
+  <si>
+    <t>BAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check the order by </t>
+  </si>
+  <si>
+    <t>Click on " Cart" button</t>
+  </si>
+  <si>
+    <t>While user click on " Cart" button it should be open the Bag and show the all add to cart product</t>
+  </si>
+  <si>
+    <t>Click on " Cancel" bar</t>
+  </si>
+  <si>
+    <t>While user click on " Cancel" bar it should be product remove the add to cart list.</t>
+  </si>
+  <si>
+    <t>Click on " plus(+)"</t>
+  </si>
+  <si>
+    <t>While user click on plus(+), it should be increase the product quantity</t>
+  </si>
+  <si>
+    <t>Click on " minus(-)</t>
+  </si>
+  <si>
+    <t>While uset click on minus(-), it should be decrease the product quantity</t>
+  </si>
+  <si>
+    <t>Click on " Checkout"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">While user click on CHECKOUT button, it should be open the shipping address details </t>
+  </si>
+  <si>
+    <t>Check the " Submit" button</t>
+  </si>
+  <si>
+    <t>While user enter the first name, last name, address, state, postal code then click on Submit button it should be open the confirmation page.</t>
+  </si>
+  <si>
+    <t>Check the Download receipt</t>
+  </si>
+  <si>
+    <t>While user click on Download receipt it should be download the order receipt on your phone</t>
+  </si>
+  <si>
+    <t>Check the Continuous Shopping</t>
+  </si>
+  <si>
+    <t>While user click on " Continuous Shopping" It should be redirect to the Home page.</t>
+  </si>
+  <si>
+    <t>Check the Logout button</t>
+  </si>
+  <si>
+    <t>While user click on logout button, it should be logout the account</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -539,24 +508,8 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -596,7 +549,6 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -604,15 +556,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -931,7 +886,7 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,25 +896,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -967,10 +922,10 @@
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>41</v>
       </c>
     </row>
@@ -978,10 +933,10 @@
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>42</v>
       </c>
     </row>
@@ -989,10 +944,10 @@
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1000,10 +955,10 @@
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1011,10 +966,10 @@
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1022,10 +977,10 @@
       <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1033,10 +988,10 @@
       <c r="A10">
         <v>7</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1044,10 +999,10 @@
       <c r="A11">
         <v>8</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1055,10 +1010,10 @@
       <c r="A12">
         <v>9</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1066,10 +1021,10 @@
       <c r="A13">
         <v>10</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1077,10 +1032,10 @@
       <c r="A14">
         <v>11</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1088,10 +1043,10 @@
       <c r="A15">
         <v>12</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1099,10 +1054,10 @@
       <c r="A16">
         <v>13</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1110,10 +1065,10 @@
       <c r="A17">
         <v>14</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1121,10 +1076,10 @@
       <c r="A18">
         <v>15</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1132,10 +1087,10 @@
       <c r="A19">
         <v>16</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1143,10 +1098,10 @@
       <c r="A20">
         <v>17</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1154,10 +1109,10 @@
       <c r="A21">
         <v>18</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1165,10 +1120,10 @@
       <c r="A22">
         <v>19</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1176,10 +1131,10 @@
       <c r="A23">
         <v>20</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1187,10 +1142,10 @@
       <c r="A24">
         <v>20</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1198,10 +1153,10 @@
       <c r="A25">
         <v>21</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1209,10 +1164,10 @@
       <c r="A26">
         <v>22</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1220,10 +1175,10 @@
       <c r="A27">
         <v>22</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1231,10 +1186,10 @@
       <c r="A28">
         <v>23</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1242,10 +1197,10 @@
       <c r="A29">
         <v>24</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1253,10 +1208,10 @@
       <c r="A30">
         <v>25</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1264,10 +1219,10 @@
       <c r="A31">
         <v>26</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1275,10 +1230,10 @@
       <c r="A32">
         <v>27</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1286,10 +1241,10 @@
       <c r="A33">
         <v>28</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1297,10 +1252,10 @@
       <c r="A34">
         <v>29</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1308,10 +1263,10 @@
       <c r="A35">
         <v>30</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1319,10 +1274,10 @@
       <c r="A36">
         <v>31</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1330,10 +1285,10 @@
       <c r="A37">
         <v>32</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1344,7 +1299,7 @@
       <c r="B38" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="2" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1352,28 +1307,28 @@
       <c r="A39">
         <v>34</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="3"/>
+      <c r="C39" s="2"/>
     </row>
     <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>35</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="3"/>
+      <c r="C40" s="2"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>36</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C41" s="3"/>
+      <c r="C41" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1384,536 +1339,474 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{212DF483-DA44-4D9E-86C5-E5DD46985B2B}">
-  <dimension ref="A1:C23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B9454E-7404-4B68-A525-472ABF1ECCAF}">
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" customWidth="1"/>
-    <col min="3" max="3" width="68.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="B5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>86</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>94</v>
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="16" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C20" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C16" s="3" t="s">
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>16</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C21" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>18</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>19</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>19.2</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>20</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>108</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>110</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>112</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>114</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="C28" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>20.2</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="C29" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>20.3</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
-        <v>116</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="B31" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>21.1</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+    </row>
+    <row r="36" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
-        <v>121</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>122</v>
+      <c r="B36" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>22.1</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>22.2</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>22.3</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>22.4</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>23</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>24</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>25</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>26</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A18:C19"/>
+    <mergeCell ref="A34:C35"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B9454E-7404-4B68-A525-472ABF1ECCAF}">
-  <dimension ref="A1:C23"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="41.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-    </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>15</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>16</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>17</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>18</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A18:C19"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3529B7A6-B0F3-4BC0-96AC-176FC0943A8F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1922,7 +1815,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D565A5-634D-441D-B800-DE46C042804A}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>